<commit_message>
Lista empresas orçamento Registradores
</commit_message>
<xml_diff>
--- a/hardware/registradores/docs/orcamento.xlsx
+++ b/hardware/registradores/docs/orcamento.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FC3E85FB-3083-4854-9520-F3B90CFCB86C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A42CF125-F5DC-4F1C-B203-297FEEF69E6F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCIs" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>Dimensão (mm x mm)</t>
   </si>
   <si>
-    <t>REV20180903</t>
-  </si>
-  <si>
     <t>Projeto</t>
   </si>
   <si>
@@ -96,13 +93,136 @@
   </si>
   <si>
     <t>Nova Trento - SC</t>
+  </si>
+  <si>
+    <t>Prazo</t>
+  </si>
+  <si>
+    <t>Circuitel</t>
+  </si>
+  <si>
+    <t>Pinhais - PR</t>
+  </si>
+  <si>
+    <t>vendas@circuitel.com.br</t>
+  </si>
+  <si>
+    <t>Menor isolação (mil)</t>
+  </si>
+  <si>
+    <t>Menor pista (mil)</t>
+  </si>
+  <si>
+    <t>Diâmetro do menor furo (mil)</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>NV Tecnologia</t>
+  </si>
+  <si>
+    <t> nvtecnologia@plugnet.com.br ; altair@nvtecnologia.com.br</t>
+  </si>
+  <si>
+    <t>Griffus</t>
+  </si>
+  <si>
+    <t>Cotia - SP</t>
+  </si>
+  <si>
+    <t>gvendas@griffus.com.br</t>
+  </si>
+  <si>
+    <t>Tecnel</t>
+  </si>
+  <si>
+    <t>Taboão da Serra - SP</t>
+  </si>
+  <si>
+    <t>vendas@tecneleletronica.com.br</t>
+  </si>
+  <si>
+    <t>Rossi-Plac</t>
+  </si>
+  <si>
+    <t>vendas@rossiplac.com </t>
+  </si>
+  <si>
+    <t>AMR Eletrônica</t>
+  </si>
+  <si>
+    <t>contato@amreletronica.com.br</t>
+  </si>
+  <si>
+    <t>Stick</t>
+  </si>
+  <si>
+    <t>Belo Horizonte - MG</t>
+  </si>
+  <si>
+    <t>stick@stick.ind.br</t>
+  </si>
+  <si>
+    <t>Cirvale</t>
+  </si>
+  <si>
+    <t>Sta Rita do Sapucaí - MG</t>
+  </si>
+  <si>
+    <t>orcamento@cirvale.com.br</t>
+  </si>
+  <si>
+    <t>WF</t>
+  </si>
+  <si>
+    <t>Presidente Prudente - SP</t>
+  </si>
+  <si>
+    <t>wf@wf.ind.br</t>
+  </si>
+  <si>
+    <t>https://curtacircuitos.com.br/</t>
+  </si>
+  <si>
+    <t>Luchtec</t>
+  </si>
+  <si>
+    <t>Guarulhos - SP</t>
+  </si>
+  <si>
+    <t>contato@luchtec.com.br</t>
+  </si>
+  <si>
+    <t>RCI</t>
+  </si>
+  <si>
+    <t>Osasco - SP</t>
+  </si>
+  <si>
+    <t>vendas@rcicircuitos.com.br</t>
+  </si>
+  <si>
+    <t>Printcir</t>
+  </si>
+  <si>
+    <t>print@printcir.com.br</t>
+  </si>
+  <si>
+    <t>REV20180906</t>
+  </si>
+  <si>
+    <t>FR4 dupla-face</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +245,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -173,6 +299,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -454,127 +590,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="8"/>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B5" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>23</v>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3">
+        <v>28</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{C1524448-0A69-48D2-A18A-06AD1AFE6651}"/>
-    <hyperlink ref="F3" r:id="rId2" display="mailto:vbcircuitos@vbcircuitos.com.br" xr:uid="{B2A6193A-86B0-4D38-8E29-DD1220E7951F}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{C37F39E3-9FDE-48F2-987C-D43976E5B17E}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{544F16F1-9463-4BD0-9757-A1DD05B5A8ED}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{C1524448-0A69-48D2-A18A-06AD1AFE6651}"/>
+    <hyperlink ref="G3" r:id="rId2" display="mailto:vbcircuitos@vbcircuitos.com.br" xr:uid="{B2A6193A-86B0-4D38-8E29-DD1220E7951F}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{C37F39E3-9FDE-48F2-987C-D43976E5B17E}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{544F16F1-9463-4BD0-9757-A1DD05B5A8ED}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{8B699A65-4127-45B3-8ED2-592013A1F940}"/>
+    <hyperlink ref="G4" r:id="rId6" display="mailto:%20nvtecnologia@plugnet.com.br%20;%20altair@nvtecnologia.com.br" xr:uid="{7CC45941-682A-4BB5-8BDB-E60B28A05981}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{C484C64E-A186-4805-AC9E-6A87D7AEE81C}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{3AB3E960-3E12-43DB-8782-334F0FAC3FD0}"/>
+    <hyperlink ref="G12" r:id="rId9" xr:uid="{33794266-9649-4CAB-A5BE-C716E16C9D88}"/>
+    <hyperlink ref="G13" r:id="rId10" xr:uid="{63CD2852-93F6-4D7F-BF57-EA645B9DB4EF}"/>
+    <hyperlink ref="G15" r:id="rId11" xr:uid="{A2529BB8-B65F-4CE5-9EFC-1D7179D9CB77}"/>
+    <hyperlink ref="G16" r:id="rId12" xr:uid="{8A2DD311-71A2-4081-ABE9-E27775B145EB}"/>
+    <hyperlink ref="G17" r:id="rId13" xr:uid="{5791D631-9CE6-485D-9925-70FDBF598483}"/>
+    <hyperlink ref="G9" r:id="rId14" xr:uid="{70E1DC4D-76E8-4FB9-A63A-7156B5A56D89}"/>
+    <hyperlink ref="G10" r:id="rId15" xr:uid="{83A80A09-E873-45DC-90FC-DEAA46CC3410}"/>
+    <hyperlink ref="G14" r:id="rId16" xr:uid="{4128FA31-E919-448A-924E-C7F5CD56561E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -582,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC179007-8CAF-4FA5-93C5-FBC7D88E4E77}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>